<commit_message>
Change PWM generation IC package to TSSOP due to availibility
</commit_message>
<xml_diff>
--- a/FlySensei_Stack_Actuation_ECAD/BOM/FlySensei_Stack_Actuation_ECAD_BOM.xlsx
+++ b/FlySensei_Stack_Actuation_ECAD/BOM/FlySensei_Stack_Actuation_ECAD_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph/Onedrive_JPM/OneDrive - George Mason University/Classwork/Research/Project_BlimpSquad/PCB/FlySensei_Stack_ECAD/FlySensei_Stack_Actuation_ECAD/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exchangelabsgmu-my.sharepoint.com/personal/jprincem_masonlive_gmu_edu/Documents/Classwork/Research/Project_BlimpSquad/PCB/FlySensei_Stack_ECAD/FlySensei_Stack_Actuation_ECAD/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E5C491-BA0E-A349-BCD8-1EB7BA9EA5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{03E5C491-BA0E-A349-BCD8-1EB7BA9EA5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E56AD0E-0F71-DC49-AAC5-F8A3633DC88F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,9 +324,6 @@
     <t>NXP</t>
   </si>
   <si>
-    <t>PCA9685BS,118</t>
-  </si>
-  <si>
     <t>IC LED DRVR LIN DIM 25MA 28HVQFN</t>
   </si>
   <si>
@@ -345,12 +342,6 @@
     <t>Maxim Integrated</t>
   </si>
   <si>
-    <t>MAX17049G+T10</t>
-  </si>
-  <si>
-    <t>IC BATT MON LI-ION 2CELL 8TDFN</t>
-  </si>
-  <si>
     <t>8-TDFN</t>
   </si>
   <si>
@@ -376,6 +367,15 @@
   </si>
   <si>
     <t xml:space="preserve">Package/Footprint </t>
+  </si>
+  <si>
+    <t>PCA9685PW,118</t>
+  </si>
+  <si>
+    <t>MAX17059G+</t>
+  </si>
+  <si>
+    <t>IC BATT FUEL LI-ION 2C 8TDFN</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -822,22 +822,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>3</v>
@@ -1481,13 +1481,13 @@
         <v>99</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="G25" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>102</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>6</v>
@@ -1508,13 +1508,13 @@
         <v>41</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="G26" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>105</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>6</v>
@@ -1541,7 +1541,7 @@
         <v>44</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>6</v>
@@ -1559,16 +1559,16 @@
         <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>6</v>
@@ -1589,13 +1589,13 @@
         <v>41</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>6</v>

</xml_diff>